<commit_message>
can now specify font size in meta_table
</commit_message>
<xml_diff>
--- a/inst/extdata/meta_table.xlsx
+++ b/inst/extdata/meta_table.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>Completed</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>1.1</t>
+  </si>
+  <si>
+    <t>fontsize</t>
   </si>
 </sst>
 </file>
@@ -937,15 +940,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1000,8 +1003,11 @@
       <c r="R1" t="s">
         <v>17</v>
       </c>
+      <c r="S1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1032,8 +1038,11 @@
       <c r="Q2" t="s">
         <v>31</v>
       </c>
+      <c r="S2">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1064,8 +1073,11 @@
       <c r="Q3" t="s">
         <v>31</v>
       </c>
+      <c r="S3">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1098,6 +1110,9 @@
       </c>
       <c r="O4" t="s">
         <v>24</v>
+      </c>
+      <c r="S4">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>